<commit_message>
Second Run for Stock Price Prediction ML project w Basic RF
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,67 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>model score</t>
+          <t>current_close</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>delta pred</t>
+          <t>pred_30d</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>delta_pred</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>R2 (Train)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>R2 (Test)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MSE (Train)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MSE (Val)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MSE (Test)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE (Train)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE (Test)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>DA (Train)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>DA (Test)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>DA (Val)</t>
         </is>
       </c>
     </row>
@@ -456,11 +511,70 @@
           <t>AMZN</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0.9346715345839693</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.081938886014528</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>235.06</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>228.92</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.9739</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.9894</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-0.7561</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5.0716</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>852.3893</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>147.3108</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2.2520</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>12.1372</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.9756</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0.6458</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.4583</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -469,11 +583,70 @@
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.9432564791117274</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.040710027524013</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>271.05</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>234.91</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.8667</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.9917</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-0.1860</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5.2864</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>425.8522</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>548.3502</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2.2992</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>23.4169</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.9373</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.7188</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.4062</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -482,11 +655,70 @@
           <t>GOOG</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.9456648353867716</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.115237952599248</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>271.89</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>185.91</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.6837</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.9858</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-2.9357</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4.4201</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>144.9006</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>4511.4090</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2.1024</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>67.1670</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>0.9721</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>0.2083</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0.7917</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -495,11 +727,70 @@
           <t>NDAQ</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0.9820795619601602</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.9967218178737005</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>87.24</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>79.62</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.9127</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.9950</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-12.8617</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.3956</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>37.6962</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>167.0369</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.6290</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>12.9243</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.9582</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.5000</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.7917</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -508,11 +799,70 @@
           <t>META</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0.8963398869800393</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8680800974762097</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>601.79</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>600.31</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.9975</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.9906</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-5.2438</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>56.8423</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>9540.9640</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>11328.5530</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>7.5394</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>106.4357</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.9721</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.5312</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.6771</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -521,11 +871,70 @@
           <t>TSLA</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.9312109508666139</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.9204904368004672</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>386.30</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>392.42</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.0158</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.9820</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-0.0089</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>122.4193</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>12071.9840</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3336.2968</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>11.0643</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>57.7607</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>0.9512</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>0.6458</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0.5312</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -534,11 +943,70 @@
           <t>INTC</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.9366030624543734</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.990236148703376</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>35.03</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>23.38</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.6673</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.9934</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-0.9215</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.6310</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>6.2321</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>97.6837</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.7943</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>9.8835</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>0.9443</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>0.5625</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.7812</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -547,11 +1015,70 @@
           <t>AMD</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0.8628223645171536</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.408122928001069</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>240.11</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>139.70</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.5818</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.9720</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-1.0489</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>11.9261</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>3041.3938</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3028.8064</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>3.4534</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>55.0346</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>0.9652</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>0.5833</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0.4167</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>